<commit_message>
0.0.14 v3.0 + docs
</commit_message>
<xml_diff>
--- a/Project Outputs for dv_analog/BOM/dv_analog.xlsx
+++ b/Project Outputs for dv_analog/BOM/dv_analog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26115" windowHeight="15345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26100" windowHeight="15345"/>
   </bookViews>
   <sheets>
     <sheet name="dv_analog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t>Designator</t>
   </si>
@@ -116,58 +116,64 @@
     <t>R24, R43, R62, R81, R100, R119</t>
   </si>
   <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>R23, R42, R61, R80, R99, R118</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R22, R41, R60, R79, R98, R117</t>
+  </si>
+  <si>
+    <t>NU*</t>
+  </si>
+  <si>
+    <t>R20, R39, R58, R77, R96, R115</t>
+  </si>
+  <si>
+    <t>5к</t>
+  </si>
+  <si>
+    <t>R17, R36, R55, R74, R93, R112</t>
+  </si>
+  <si>
     <t>110k</t>
   </si>
   <si>
-    <t>R22, R41, R60, R79, R98, R117</t>
+    <t>R15, R34, R53, R72, R91, R110</t>
   </si>
   <si>
     <t>22k</t>
   </si>
   <si>
-    <t>R17, R36, R55, R74, R93, R112</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>R16, R35, R54, R73, R92, R111</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R15, R34, R53, R72, R91, R110</t>
-  </si>
-  <si>
-    <t>NU*</t>
-  </si>
-  <si>
-    <t>R13, R20, R32, R39, R51, R58, R70, R77, R89, R96, R108, R115</t>
-  </si>
-  <si>
-    <t>200к</t>
+    <t>R14, R21, R33, R40, R52, R59, R71, R78, R90, R97, R109, R116</t>
+  </si>
+  <si>
+    <t>13k3</t>
+  </si>
+  <si>
+    <t>R13, R32, R51, R70, R89, R108</t>
+  </si>
+  <si>
+    <t>20к</t>
   </si>
   <si>
     <t>R12, R19, R31, R38, R50, R57, R69, R76, R88, R95, R107, R114</t>
   </si>
   <si>
-    <t>2k15</t>
-  </si>
-  <si>
-    <t>R11, R14, R18, R21, R30, R33, R37, R40, R49, R52, R56, R59, R68, R71, R75, R78, R87, R90, R94, R97, R106, R109, R113, R116</t>
-  </si>
-  <si>
-    <t>3k9</t>
-  </si>
-  <si>
-    <t>R10, R29, R48, R67, R86, R105</t>
-  </si>
-  <si>
-    <t>51k</t>
-  </si>
-  <si>
-    <t>R8, R9, R23, R27, R28, R42, R46, R47, R61, R65, R66, R80, R84, R85, R99, R103, R104, R118</t>
+    <t>8k2</t>
+  </si>
+  <si>
+    <t>R11, R18, R30, R37, R49, R56, R68, R75, R87, R94, R106, R113</t>
+  </si>
+  <si>
+    <t>27k</t>
+  </si>
+  <si>
+    <t>R8, R9, R16, R27, R28, R35, R46, R47, R54, R65, R66, R73, R84, R85, R92, R103, R104, R111</t>
   </si>
   <si>
     <t>330</t>
@@ -182,7 +188,13 @@
     <t>R6</t>
   </si>
   <si>
-    <t>2k</t>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>3k6</t>
   </si>
   <si>
     <t>R4</t>
@@ -194,10 +206,10 @@
     <t>R3</t>
   </si>
   <si>
-    <t>820</t>
-  </si>
-  <si>
-    <t>R1, R2, R5</t>
+    <t>1k6</t>
+  </si>
+  <si>
+    <t>R1, R2, R10, R29, R48, R67, R86, R105</t>
   </si>
   <si>
     <t>1k</t>
@@ -224,15 +236,21 @@
     <t>К10-79</t>
   </si>
   <si>
+    <t>4.7 пФ</t>
+  </si>
+  <si>
+    <t>C16_dv_analog_interface_ch1, C16_dv_analog_interface_ch2, C16_dv_analog_interface_ch3, C16_dv_analog_interface_ch4, C16_dv_analog_interface_ch5, C16_dv_analog_interface_ch6</t>
+  </si>
+  <si>
+    <t>10 нФ</t>
+  </si>
+  <si>
+    <t>C13, C26, C39, C52, C65, C78</t>
+  </si>
+  <si>
     <t>24 пФ</t>
   </si>
   <si>
-    <t>C13, C26, C39, C52, C65, C78</t>
-  </si>
-  <si>
-    <t>4.7 пФ</t>
-  </si>
-  <si>
     <t>C12, C16, C25, C29, C38, C42, C51, C55, C64, C68, C77, C81</t>
   </si>
   <si>
@@ -242,7 +260,7 @@
     <t>C9, C22, C35, C48, C61, C74</t>
   </si>
   <si>
-    <t>150пФ</t>
+    <t>8200пФ</t>
   </si>
   <si>
     <t>C7, C8, C10, C11, C14, C15, C18, C19, C20, C21, C23, C24, C27, C28, C31, C32, C33, C34, C36, C37, C40, C41, C44, C45, C46, C47, C49, C50, C53, C54, C57, C58, C59, C60, C62, C63, C66, C67, C70, C71, C72, C73, C75, C76, C79, C80, C83, C84</t>
@@ -616,7 +634,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -862,7 +880,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>39</v>
@@ -896,7 +914,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>43</v>
@@ -913,7 +931,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="1">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>45</v>
@@ -930,7 +948,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>47</v>
@@ -947,7 +965,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>49</v>
@@ -1015,7 +1033,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>57</v>
@@ -1026,38 +1044,38 @@
         <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D26" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>63</v>
@@ -1066,24 +1084,24 @@
         <v>64</v>
       </c>
       <c r="D27" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D28" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>69</v>
@@ -1094,10 +1112,10 @@
         <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1">
         <v>6</v>
@@ -1111,13 +1129,13 @@
         <v>72</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>73</v>
@@ -1128,13 +1146,13 @@
         <v>74</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>75</v>
@@ -1145,33 +1163,84 @@
         <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="1">
-        <v>2</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="1">
+        <v>48</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="B34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="1">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1">
         <v>1</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>81</v>
+      <c r="E36" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>